<commit_message>
Completed group SRS and group work schedule.
</commit_message>
<xml_diff>
--- a/Documents/BazingaWorkSchedule.xlsx
+++ b/Documents/BazingaWorkSchedule.xlsx
@@ -1285,13 +1285,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1303,195 +1296,20 @@
     <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="102">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="51">
     <dxf>
       <fill>
         <patternFill>
@@ -1893,266 +1711,6 @@
       <fill>
         <patternFill>
           <bgColor indexed="40"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="23"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="44"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3925,8 +3483,8 @@
   </sheetPr>
   <dimension ref="A1:IV66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3954,12 +3512,12 @@
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
       <c r="K1" s="51">
         <v>0</v>
       </c>
@@ -4003,10 +3561,10 @@
       <c r="F2" s="52"/>
       <c r="G2" s="52"/>
       <c r="H2" s="52"/>
-      <c r="I2" s="81" t="s">
+      <c r="I2" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="81"/>
+      <c r="J2" s="79"/>
     </row>
     <row r="3" spans="1:256" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
@@ -4020,11 +3578,11 @@
       <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="78">
+      <c r="H4" s="81">
         <v>40942</v>
       </c>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
       <c r="K4" s="55" t="str">
         <f>TEXT(H4,"dddd")</f>
         <v>Friday</v>
@@ -4039,11 +3597,11 @@
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="80" t="s">
+      <c r="C6" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="IQ6" s="18" t="s">
@@ -4054,10 +3612,10 @@
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="79">
+      <c r="C7" s="77">
         <v>40913</v>
       </c>
-      <c r="D7" s="79"/>
+      <c r="D7" s="77"/>
       <c r="E7" s="55" t="str">
         <f>TEXT(C7,"dddd")</f>
         <v>Thursday</v>
@@ -10809,7 +10367,7 @@
       </c>
       <c r="G29" s="25">
         <f>SUMPRODUCT(F31:F38,G31:G38)/SUM(F31:F38)</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0.21176470588235294</v>
       </c>
       <c r="H29" s="71">
         <f t="shared" si="4"/>
@@ -10817,11 +10375,11 @@
       </c>
       <c r="I29" s="72">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J29" s="71">
         <f t="shared" si="6"/>
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="IP29" s="62"/>
       <c r="IQ29" s="62"/>
@@ -11126,17 +10684,17 @@
       </c>
       <c r="E31" s="65">
         <f t="shared" ref="E31:E47" si="31">D31+F31-1</f>
-        <v>40990</v>
+        <v>40969</v>
       </c>
       <c r="F31" s="29">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="G31" s="30">
         <v>0</v>
       </c>
       <c r="H31" s="66">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I31" s="67">
         <f t="shared" si="5"/>
@@ -11144,7 +10702,7 @@
       </c>
       <c r="J31" s="66">
         <f t="shared" si="6"/>
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="K31" s="68"/>
       <c r="L31" s="68"/>
@@ -11407,17 +10965,17 @@
       </c>
       <c r="E32" s="65">
         <f>D32+F32-1</f>
-        <v>40990</v>
+        <v>40955</v>
       </c>
       <c r="F32" s="29">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="G32" s="30">
         <v>0</v>
       </c>
       <c r="H32" s="66">
         <f>NETWORKDAYS(D32,E32)</f>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="I32" s="67">
         <f t="shared" ref="I32" si="32">ROUNDDOWN(G32*F32,0)</f>
@@ -11425,7 +10983,7 @@
       </c>
       <c r="J32" s="66">
         <f t="shared" ref="J32" si="33">F32-I32</f>
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="K32" s="68"/>
       <c r="L32" s="68"/>
@@ -11688,17 +11246,17 @@
       </c>
       <c r="E33" s="65">
         <f t="shared" ref="E33" si="34">D33+F33-1</f>
-        <v>40990</v>
+        <v>40955</v>
       </c>
       <c r="F33" s="29">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="G33" s="30">
         <v>0</v>
       </c>
       <c r="H33" s="66">
         <f t="shared" ref="H33" si="35">NETWORKDAYS(D33,E33)</f>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="I33" s="67">
         <f t="shared" ref="I33" si="36">ROUNDDOWN(G33*F33,0)</f>
@@ -11706,7 +11264,7 @@
       </c>
       <c r="J33" s="66">
         <f t="shared" ref="J33" si="37">F33-I33</f>
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="K33" s="68"/>
       <c r="L33" s="68"/>
@@ -11969,17 +11527,17 @@
       </c>
       <c r="E34" s="65">
         <f t="shared" ref="E34:E35" si="38">D34+F34-1</f>
-        <v>40990</v>
+        <v>40955</v>
       </c>
       <c r="F34" s="29">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="G34" s="30">
         <v>0</v>
       </c>
       <c r="H34" s="66">
         <f t="shared" ref="H34:H35" si="39">NETWORKDAYS(D34,E34)</f>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="I34" s="67">
         <f t="shared" ref="I34" si="40">ROUNDDOWN(G34*F34,0)</f>
@@ -11987,7 +11545,7 @@
       </c>
       <c r="J34" s="66">
         <f t="shared" ref="J34" si="41">F34-I34</f>
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="K34" s="68"/>
       <c r="L34" s="68"/>
@@ -12246,21 +11804,21 @@
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="28">
-        <v>40949</v>
+        <v>40971</v>
       </c>
       <c r="E35" s="65">
         <f t="shared" si="38"/>
-        <v>40990</v>
+        <v>40984</v>
       </c>
       <c r="F35" s="29">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G35" s="30">
         <v>0</v>
       </c>
       <c r="H35" s="66">
         <f t="shared" si="39"/>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I35" s="67">
         <f>ROUNDDOWN(G35*F35,0)</f>
@@ -12268,7 +11826,7 @@
       </c>
       <c r="J35" s="66">
         <f>F35-I35</f>
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="K35" s="68"/>
       <c r="L35" s="68"/>
@@ -12527,21 +12085,21 @@
       </c>
       <c r="C36" s="27"/>
       <c r="D36" s="28">
-        <v>40949</v>
+        <v>40971</v>
       </c>
       <c r="E36" s="65">
         <f>D36+F36-1</f>
-        <v>40990</v>
+        <v>40977</v>
       </c>
       <c r="F36" s="29">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="G36" s="30">
         <v>0</v>
       </c>
       <c r="H36" s="66">
         <f>NETWORKDAYS(D36,E36)</f>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="I36" s="67">
         <f t="shared" ref="I36:I37" si="42">ROUNDDOWN(G36*F36,0)</f>
@@ -12549,7 +12107,7 @@
       </c>
       <c r="J36" s="66">
         <f t="shared" ref="J36:J37" si="43">F36-I36</f>
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="K36" s="68"/>
       <c r="L36" s="68"/>
@@ -12808,21 +12366,21 @@
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="28">
-        <v>40949</v>
+        <v>40971</v>
       </c>
       <c r="E37" s="65">
         <f t="shared" ref="E37" si="44">D37+F37-1</f>
-        <v>40990</v>
+        <v>40984</v>
       </c>
       <c r="F37" s="29">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G37" s="30">
         <v>0</v>
       </c>
       <c r="H37" s="66">
         <f t="shared" ref="H37" si="45">NETWORKDAYS(D37,E37)</f>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I37" s="67">
         <f t="shared" si="42"/>
@@ -12830,7 +12388,7 @@
       </c>
       <c r="J37" s="66">
         <f t="shared" si="43"/>
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="K37" s="68"/>
       <c r="L37" s="68"/>
@@ -13371,7 +12929,7 @@
       <c r="C39" s="22"/>
       <c r="D39" s="23">
         <f>MIN(D40:D49)</f>
-        <v>40991</v>
+        <v>40970</v>
       </c>
       <c r="E39" s="58">
         <f t="shared" si="31"/>
@@ -13379,7 +12937,7 @@
       </c>
       <c r="F39" s="24">
         <f>MAX(E40:E49)-D39+1</f>
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="G39" s="25">
         <f>SUMPRODUCT(F40:F47,G40:G47)/SUM(F40:F47)</f>
@@ -13387,7 +12945,7 @@
       </c>
       <c r="H39" s="71">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="I39" s="72">
         <f t="shared" si="5"/>
@@ -13395,7 +12953,7 @@
       </c>
       <c r="J39" s="71">
         <f t="shared" si="6"/>
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="IP39" s="62"/>
       <c r="IQ39" s="62"/>
@@ -13411,25 +12969,25 @@
         <v>3.1</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="28">
-        <v>40991</v>
+        <v>40970</v>
       </c>
       <c r="E40" s="65">
         <f t="shared" si="31"/>
-        <v>41025</v>
+        <v>40997</v>
       </c>
       <c r="F40" s="29">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G40" s="30">
         <v>0</v>
       </c>
       <c r="H40" s="66">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I40" s="67">
         <f t="shared" si="5"/>
@@ -13437,7 +12995,7 @@
       </c>
       <c r="J40" s="66">
         <f t="shared" si="6"/>
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K40" s="68"/>
       <c r="L40" s="68"/>
@@ -13688,37 +13246,39 @@
     </row>
     <row r="41" spans="1:256" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="64" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A41,-1,0,1,1),".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",1))),OFFSET(A41,-1,0,1,1)&amp;".1",LEFT(OFFSET(A41,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",2))),VALUE(RIGHT(OFFSET(A41,-1,0,1,1),LEN(OFFSET(A41,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",1))))+1,VALUE(MID(OFFSET(A41,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",1))+1,(FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",2))-FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",1))-1)))+1)))</f>
-        <v>3.2</v>
-      </c>
-      <c r="B41" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="27"/>
+        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A41,-1,0,1,1),".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",3))),OFFSET(A41,-1,0,1,1)&amp;".1",LEFT(OFFSET(A41,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",4))),VALUE(RIGHT(OFFSET(A41,-1,0,1,1),LEN(OFFSET(A41,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",3))))+1,VALUE(MID(OFFSET(A41,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",3))+1,(FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",4))-FIND("`",SUBSTITUTE(OFFSET(A41,-1,0,1,1),".","`",3))-1)))+1)))</f>
+        <v>3.1.1</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>63</v>
+      </c>
       <c r="D41" s="28">
-        <v>40991</v>
+        <v>40970</v>
       </c>
       <c r="E41" s="65">
         <f t="shared" si="31"/>
-        <v>41025</v>
+        <v>40997</v>
       </c>
       <c r="F41" s="29">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G41" s="30">
         <v>0</v>
       </c>
       <c r="H41" s="66">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I41" s="67">
-        <f t="shared" si="5"/>
+        <f>ROUNDDOWN(G41*F41,0)</f>
         <v>0</v>
       </c>
       <c r="J41" s="66">
-        <f t="shared" si="6"/>
-        <v>35</v>
+        <f>F41-I41</f>
+        <v>28</v>
       </c>
       <c r="K41" s="68"/>
       <c r="L41" s="68"/>
@@ -13970,30 +13530,30 @@
     <row r="42" spans="1:256" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="64" t="str">
         <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A42,-1,0,1,1),".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A42,-1,0,1,1),".","`",3))),OFFSET(A42,-1,0,1,1)&amp;".1",LEFT(OFFSET(A42,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A42,-1,0,1,1),".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A42,-1,0,1,1),".","`",4))),VALUE(RIGHT(OFFSET(A42,-1,0,1,1),LEN(OFFSET(A42,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A42,-1,0,1,1),".","`",3))))+1,VALUE(MID(OFFSET(A42,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A42,-1,0,1,1),".","`",3))+1,(FIND("`",SUBSTITUTE(OFFSET(A42,-1,0,1,1),".","`",4))-FIND("`",SUBSTITUTE(OFFSET(A42,-1,0,1,1),".","`",3))-1)))+1)))</f>
-        <v>3.2.1</v>
+        <v>3.1.1.1</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="D42" s="28">
-        <v>40991</v>
+        <v>40970</v>
       </c>
       <c r="E42" s="65">
         <f t="shared" si="31"/>
-        <v>41025</v>
+        <v>40997</v>
       </c>
       <c r="F42" s="29">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G42" s="30">
         <v>0</v>
       </c>
       <c r="H42" s="66">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I42" s="67">
         <f>ROUNDDOWN(G42*F42,0)</f>
@@ -14001,7 +13561,7 @@
       </c>
       <c r="J42" s="66">
         <f>F42-I42</f>
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K42" s="68"/>
       <c r="L42" s="68"/>
@@ -14253,30 +13813,30 @@
     <row r="43" spans="1:256" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="64" t="str">
         <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A43,-1,0,1,1),".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A43,-1,0,1,1),".","`",3))),OFFSET(A43,-1,0,1,1)&amp;".1",LEFT(OFFSET(A43,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A43,-1,0,1,1),".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A43,-1,0,1,1),".","`",4))),VALUE(RIGHT(OFFSET(A43,-1,0,1,1),LEN(OFFSET(A43,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A43,-1,0,1,1),".","`",3))))+1,VALUE(MID(OFFSET(A43,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A43,-1,0,1,1),".","`",3))+1,(FIND("`",SUBSTITUTE(OFFSET(A43,-1,0,1,1),".","`",4))-FIND("`",SUBSTITUTE(OFFSET(A43,-1,0,1,1),".","`",3))-1)))+1)))</f>
-        <v>3.2.1.1</v>
+        <v>3.1.1.2</v>
       </c>
       <c r="B43" s="35" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D43" s="28">
-        <v>40991</v>
+        <v>40970</v>
       </c>
       <c r="E43" s="65">
         <f t="shared" si="31"/>
-        <v>41025</v>
+        <v>40997</v>
       </c>
       <c r="F43" s="29">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G43" s="30">
         <v>0</v>
       </c>
       <c r="H43" s="66">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I43" s="67">
         <f>ROUNDDOWN(G43*F43,0)</f>
@@ -14284,7 +13844,7 @@
       </c>
       <c r="J43" s="66">
         <f>F43-I43</f>
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K43" s="68"/>
       <c r="L43" s="68"/>
@@ -14536,30 +14096,30 @@
     <row r="44" spans="1:256" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="64" t="str">
         <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A44,-1,0,1,1),".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A44,-1,0,1,1),".","`",3))),OFFSET(A44,-1,0,1,1)&amp;".1",LEFT(OFFSET(A44,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A44,-1,0,1,1),".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A44,-1,0,1,1),".","`",4))),VALUE(RIGHT(OFFSET(A44,-1,0,1,1),LEN(OFFSET(A44,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A44,-1,0,1,1),".","`",3))))+1,VALUE(MID(OFFSET(A44,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A44,-1,0,1,1),".","`",3))+1,(FIND("`",SUBSTITUTE(OFFSET(A44,-1,0,1,1),".","`",4))-FIND("`",SUBSTITUTE(OFFSET(A44,-1,0,1,1),".","`",3))-1)))+1)))</f>
-        <v>3.2.1.2</v>
+        <v>3.1.1.3</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="D44" s="28">
-        <v>40991</v>
+        <v>40970</v>
       </c>
       <c r="E44" s="65">
         <f t="shared" si="31"/>
-        <v>41025</v>
+        <v>40997</v>
       </c>
       <c r="F44" s="29">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G44" s="30">
         <v>0</v>
       </c>
       <c r="H44" s="66">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I44" s="67">
         <f>ROUNDDOWN(G44*F44,0)</f>
@@ -14567,7 +14127,7 @@
       </c>
       <c r="J44" s="66">
         <f>F44-I44</f>
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K44" s="68"/>
       <c r="L44" s="68"/>
@@ -14819,30 +14379,30 @@
     <row r="45" spans="1:256" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="64" t="str">
         <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A45,-1,0,1,1),".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A45,-1,0,1,1),".","`",3))),OFFSET(A45,-1,0,1,1)&amp;".1",LEFT(OFFSET(A45,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A45,-1,0,1,1),".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A45,-1,0,1,1),".","`",4))),VALUE(RIGHT(OFFSET(A45,-1,0,1,1),LEN(OFFSET(A45,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A45,-1,0,1,1),".","`",3))))+1,VALUE(MID(OFFSET(A45,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A45,-1,0,1,1),".","`",3))+1,(FIND("`",SUBSTITUTE(OFFSET(A45,-1,0,1,1),".","`",4))-FIND("`",SUBSTITUTE(OFFSET(A45,-1,0,1,1),".","`",3))-1)))+1)))</f>
-        <v>3.2.1.3</v>
+        <v>3.1.1.4</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D45" s="28">
-        <v>40991</v>
+        <v>40970</v>
       </c>
       <c r="E45" s="65">
         <f t="shared" si="31"/>
-        <v>41025</v>
+        <v>40997</v>
       </c>
       <c r="F45" s="29">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G45" s="30">
         <v>0</v>
       </c>
       <c r="H45" s="66">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I45" s="67">
         <f>ROUNDDOWN(G45*F45,0)</f>
@@ -14850,7 +14410,7 @@
       </c>
       <c r="J45" s="66">
         <f>F45-I45</f>
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K45" s="68"/>
       <c r="L45" s="68"/>
@@ -15101,31 +14661,29 @@
     </row>
     <row r="46" spans="1:256" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="64" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A46,-1,0,1,1),".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",3))),OFFSET(A46,-1,0,1,1)&amp;".1",LEFT(OFFSET(A46,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",4))),VALUE(RIGHT(OFFSET(A46,-1,0,1,1),LEN(OFFSET(A46,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",3))))+1,VALUE(MID(OFFSET(A46,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",3))+1,(FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",4))-FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",3))-1)))+1)))</f>
-        <v>3.2.1.4</v>
-      </c>
-      <c r="B46" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>61</v>
-      </c>
+        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A46,-1,0,1,1),".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",1))),OFFSET(A46,-1,0,1,1)&amp;".1",LEFT(OFFSET(A46,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",2))),VALUE(RIGHT(OFFSET(A46,-1,0,1,1),LEN(OFFSET(A46,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",1))))+1,VALUE(MID(OFFSET(A46,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",1))+1,(FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",2))-FIND("`",SUBSTITUTE(OFFSET(A46,-1,0,1,1),".","`",1))-1)))+1)))</f>
+        <v>3.2</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="27"/>
       <c r="D46" s="28">
-        <v>40991</v>
+        <v>40970</v>
       </c>
       <c r="E46" s="65">
-        <f t="shared" si="31"/>
-        <v>41025</v>
+        <f>D46+F46-1</f>
+        <v>40997</v>
       </c>
       <c r="F46" s="29">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G46" s="30">
         <v>0</v>
       </c>
       <c r="H46" s="66">
-        <f t="shared" si="4"/>
-        <v>25</v>
+        <f>NETWORKDAYS(D46,E46)</f>
+        <v>20</v>
       </c>
       <c r="I46" s="67">
         <f>ROUNDDOWN(G46*F46,0)</f>
@@ -15133,7 +14691,7 @@
       </c>
       <c r="J46" s="66">
         <f>F46-I46</f>
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K46" s="68"/>
       <c r="L46" s="68"/>
@@ -15392,21 +14950,21 @@
       </c>
       <c r="C47" s="27"/>
       <c r="D47" s="28">
-        <v>40991</v>
+        <v>40998</v>
       </c>
       <c r="E47" s="65">
         <f t="shared" si="31"/>
         <v>41025</v>
       </c>
       <c r="F47" s="29">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G47" s="30">
         <v>0</v>
       </c>
       <c r="H47" s="66">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I47" s="67">
         <f t="shared" si="5"/>
@@ -15414,7 +14972,7 @@
       </c>
       <c r="J47" s="66">
         <f t="shared" si="6"/>
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K47" s="68"/>
       <c r="L47" s="68"/>
@@ -15673,21 +15231,21 @@
       </c>
       <c r="C48" s="27"/>
       <c r="D48" s="28">
-        <v>40991</v>
+        <v>40998</v>
       </c>
       <c r="E48" s="65">
         <f t="shared" ref="E48" si="46">D48+F48-1</f>
         <v>41025</v>
       </c>
       <c r="F48" s="29">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G48" s="30">
         <v>0</v>
       </c>
       <c r="H48" s="66">
         <f t="shared" ref="H48" si="47">NETWORKDAYS(D48,E48)</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I48" s="67">
         <f t="shared" ref="I48" si="48">ROUNDDOWN(G48*F48,0)</f>
@@ -15695,7 +15253,7 @@
       </c>
       <c r="J48" s="66">
         <f t="shared" ref="J48" si="49">F48-I48</f>
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K48" s="68"/>
       <c r="L48" s="68"/>
@@ -15954,21 +15512,21 @@
       </c>
       <c r="C49" s="27"/>
       <c r="D49" s="28">
-        <v>40991</v>
+        <v>41019</v>
       </c>
       <c r="E49" s="65">
         <f t="shared" ref="E49" si="50">D49+F49-1</f>
         <v>41025</v>
       </c>
       <c r="F49" s="29">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="G49" s="30">
         <v>0</v>
       </c>
       <c r="H49" s="66">
         <f t="shared" ref="H49" si="51">NETWORKDAYS(D49,E49)</f>
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="I49" s="67">
         <f t="shared" ref="I49" si="52">ROUNDDOWN(G49*F49,0)</f>
@@ -15976,7 +15534,7 @@
       </c>
       <c r="J49" s="66">
         <f t="shared" ref="J49" si="53">F49-I49</f>
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="K49" s="68"/>
       <c r="L49" s="68"/>
@@ -20294,29 +19852,6 @@
   </sheetData>
   <sheetProtection password="8385" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="39">
-    <mergeCell ref="EH9:EN9"/>
-    <mergeCell ref="BI9:BO9"/>
-    <mergeCell ref="EV9:FB9"/>
-    <mergeCell ref="EO9:EU9"/>
-    <mergeCell ref="EA9:EG9"/>
-    <mergeCell ref="CY9:DE9"/>
-    <mergeCell ref="DF9:DL9"/>
-    <mergeCell ref="DM9:DS9"/>
-    <mergeCell ref="DT9:DZ9"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="BB9:BH9"/>
-    <mergeCell ref="CR9:CX9"/>
-    <mergeCell ref="BP9:BV9"/>
-    <mergeCell ref="BW9:CC9"/>
-    <mergeCell ref="CD9:CJ9"/>
-    <mergeCell ref="CK9:CQ9"/>
-    <mergeCell ref="HU9:IA9"/>
-    <mergeCell ref="GS9:GY9"/>
-    <mergeCell ref="GZ9:HF9"/>
-    <mergeCell ref="HG9:HM9"/>
-    <mergeCell ref="HN9:HT9"/>
     <mergeCell ref="II9:IO9"/>
     <mergeCell ref="IB9:IH9"/>
     <mergeCell ref="G1:J1"/>
@@ -20333,270 +19868,216 @@
     <mergeCell ref="FX9:GD9"/>
     <mergeCell ref="GE9:GK9"/>
     <mergeCell ref="FC9:FI9"/>
+    <mergeCell ref="HU9:IA9"/>
+    <mergeCell ref="GS9:GY9"/>
+    <mergeCell ref="GZ9:HF9"/>
+    <mergeCell ref="HG9:HM9"/>
+    <mergeCell ref="HN9:HT9"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="BB9:BH9"/>
+    <mergeCell ref="CR9:CX9"/>
+    <mergeCell ref="BP9:BV9"/>
+    <mergeCell ref="BW9:CC9"/>
+    <mergeCell ref="CD9:CJ9"/>
+    <mergeCell ref="CK9:CQ9"/>
+    <mergeCell ref="EH9:EN9"/>
+    <mergeCell ref="BI9:BO9"/>
+    <mergeCell ref="EV9:FB9"/>
+    <mergeCell ref="EO9:EU9"/>
+    <mergeCell ref="EA9:EG9"/>
+    <mergeCell ref="CY9:DE9"/>
+    <mergeCell ref="DF9:DL9"/>
+    <mergeCell ref="DM9:DS9"/>
+    <mergeCell ref="DT9:DZ9"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="L19:IO19 L31:IO34 L40:IO41 L36:IO38 L47:IO47 L55:IO61">
-    <cfRule type="expression" dxfId="71" priority="88" stopIfTrue="1">
+  <conditionalFormatting sqref="L19:IO19 L31:IO34 L36:IO38 L55:IO61 L40:IO49">
+    <cfRule type="expression" dxfId="50" priority="88" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="89" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D19,L$8&lt;$D19+$I19)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="90" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D19,L$8&lt;=$D19+$F19-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:IO10 L29:IO29 L39:IO39 L54:IO54">
-    <cfRule type="expression" dxfId="68" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="91" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="92" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D10,L$8&lt;$D10+$I10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="93" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D10,L$8&lt;=$D10+$F10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11:IO11">
-    <cfRule type="expression" dxfId="65" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="76" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="77" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D11,L$8&lt;$D11+$I11)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="78" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D11,L$8&lt;=$D11+$F11-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12:IO13">
-    <cfRule type="expression" dxfId="62" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="73" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="74" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D12,L$8&lt;$D12+$I12)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="75" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D12,L$8&lt;=$D12+$F12-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14:IO15">
-    <cfRule type="expression" dxfId="59" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="70" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="71" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D14,L$8&lt;$D14+$I14)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="72" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D14,L$8&lt;=$D14+$F14-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:IO16">
-    <cfRule type="expression" dxfId="56" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="67" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="68" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D16,L$8&lt;$D16+$I16)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="69" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D16,L$8&lt;=$D16+$F16-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:IO18">
-    <cfRule type="expression" dxfId="53" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="64" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="65" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D17,L$8&lt;$D17+$I17)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="66" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D17,L$8&lt;=$D17+$F17-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20:IO20">
-    <cfRule type="expression" dxfId="50" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="58" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="59" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D20,L$8&lt;$D20+$I20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="60" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D20,L$8&lt;=$D20+$F20-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21:IO22">
-    <cfRule type="expression" dxfId="47" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="55" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="56" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D21,L$8&lt;$D21+$I21)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="57" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D21,L$8&lt;=$D21+$F21-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27:IO27">
-    <cfRule type="expression" dxfId="44" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="49" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="50" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D27,L$8&lt;$D27+$I27)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="51" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D27,L$8&lt;=$D27+$F27-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25:IO25">
-    <cfRule type="expression" dxfId="41" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="46" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="47" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D25,L$8&lt;$D25+$I25)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="48" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D25,L$8&lt;=$D25+$F25-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24:IO24">
-    <cfRule type="expression" dxfId="38" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="43" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="44" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D24,L$8&lt;$D24+$I24)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="45" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D24,L$8&lt;=$D24+$F24-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23:IO23">
-    <cfRule type="expression" dxfId="35" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="40" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="41" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D23,L$8&lt;$D23+$I23)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="42" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D23,L$8&lt;=$D23+$F23-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26:IO26">
-    <cfRule type="expression" dxfId="32" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="37" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="38" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D26,L$8&lt;$D26+$I26)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="39" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D26,L$8&lt;=$D26+$F26-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28:IO28">
-    <cfRule type="expression" dxfId="29" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="34" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="35" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D28,L$8&lt;$D28+$I28)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="36" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D28,L$8&lt;=$D28+$F28-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30:IO30">
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="28" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="29" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D30,L$8&lt;$D30+$I30)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="30" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D30,L$8&lt;=$D30+$F30-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35:IO35">
-    <cfRule type="expression" dxfId="23" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="25" stopIfTrue="1">
       <formula>L$8=$H$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="26" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D35,L$8&lt;$D35+$I35)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="27" stopIfTrue="1">
       <formula>AND(L$8&gt;=$D35,L$8&lt;=$D35+$F35-1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L46:IO46">
-    <cfRule type="expression" dxfId="20" priority="19" stopIfTrue="1">
-      <formula>L$8=$H$4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D46,L$8&lt;$D46+$I46)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D46,L$8&lt;=$D46+$F46-1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L44:IO44">
-    <cfRule type="expression" dxfId="17" priority="16" stopIfTrue="1">
-      <formula>L$8=$H$4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D44,L$8&lt;$D44+$I44)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D44,L$8&lt;=$D44+$F44-1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L43:IO43">
-    <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
-      <formula>L$8=$H$4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D43,L$8&lt;$D43+$I43)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D43,L$8&lt;=$D43+$F43-1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L42:IO42">
-    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
-      <formula>L$8=$H$4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D42,L$8&lt;$D42+$I42)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D42,L$8&lt;=$D42+$F42-1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L45:IO45">
-    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
-      <formula>L$8=$H$4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D45,L$8&lt;$D45+$I45)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D45,L$8&lt;=$D45+$F45-1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L48:IO48">
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
-      <formula>L$8=$H$4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D48,L$8&lt;$D48+$I48)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D48,L$8&lt;=$D48+$F48-1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L49:IO49">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
-      <formula>L$8=$H$4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D49,L$8&lt;$D49+$I49)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
-      <formula>AND(L$8&gt;=$D49,L$8&lt;=$D49+$F49-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -20608,7 +20089,7 @@
     <oddFooter>&amp;L&amp;8Gantt Chart Template by Vertex42.com&amp;R&amp;8© 2008 Vertex42 LLC</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="H54:J61 A38 A47 G54 E54:E61 H10:J10 A10 E31 H31:J31 A31 H29:J29 E38:E41 H38:J41 A40:A41 E47 H47:J47" unlockedFormula="1"/>
+    <ignoredError sqref="H54:J61 A38 A47 G54 E54:E61 H10:J10 A10 E31 H31:J31 A31 H29:J29 E38:E39 H38:J39 A40 E47 H47:J47 E40 H40:J40" unlockedFormula="1"/>
     <ignoredError sqref="A39 A29" formula="1" unlockedFormula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>

</xml_diff>